<commit_message>
fixed error - regarding git command linking local to remote
</commit_message>
<xml_diff>
--- a/help/github-command-guide.xlsx
+++ b/help/github-command-guide.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$42:$C$47</definedName>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Change name of the master branch to “main”</t>
   </si>
   <si>
-    <t xml:space="preserve">git remote add origin [repo url]</t>
+    <t xml:space="preserve">git remote add origin [repo url].git</t>
   </si>
   <si>
     <t xml:space="preserve">Link local git to github</t>
@@ -182,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,11 +219,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -307,7 +302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,10 +345,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -374,6 +365,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF3465A4"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -381,13 +373,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFDEE6EF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -395,6 +388,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -466,15 +460,121 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C69"/>
+  <dimension ref="A2:C61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,16 +810,6 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-    </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
         <v>46</v>
@@ -777,7 +867,7 @@
       <c r="B38" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -853,90 +943,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="0"/>
-      <c r="C52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
-      <c r="B53" s="0"/>
-      <c r="C53" s="0"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0"/>
-      <c r="B55" s="0"/>
-      <c r="C55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0"/>
-      <c r="B59" s="0"/>
-      <c r="C59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0"/>
-      <c r="B60" s="0"/>
-      <c r="C60" s="0"/>
-    </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0"/>
-      <c r="B63" s="0"/>
-      <c r="C63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="0"/>
-      <c r="C64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0"/>
-      <c r="B65" s="0"/>
-      <c r="C65" s="0"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0"/>
-      <c r="B66" s="0"/>
-      <c r="C66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0"/>
-      <c r="B67" s="0"/>
-      <c r="C67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="0"/>
-      <c r="C68" s="0"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A42:C47"/>

</xml_diff>